<commit_message>
add week 5 and fix format for strength sheets
</commit_message>
<xml_diff>
--- a/sam_training/program_output/Max Shethar program.xlsx
+++ b/sam_training/program_output/Max Shethar program.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Week 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Week 2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Week 3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Week 4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Week 5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -938,9 +939,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1472,9 +1475,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2006,9 +2011,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2540,9 +2547,586 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B22:E22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Week 5: Strength 1 of 3</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Exercise</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>Sets</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Reps</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Bench Press</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Lat Pulldowns (Grip of Choice)</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>8-12</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>3RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>Neutral Grip DB Bench</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>Chest Supported Row of Choice</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>8-12</t>
+        </is>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>3RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>Tricep Motion of Choice</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>12-15</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
+        <is>
+          <t>1-2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Pec Flies or Face Pulls</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>8-15</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>1-2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="n"/>
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>Exercise</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>Sets</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>Reps</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Bench Press</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="n"/>
+      <c r="C17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>Lat Pulldowns (Grip of Choice)</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>8-12</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>3RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>High Incline Neutral DB Press</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="E19" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Chest Supported Row of Choice</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>8-12</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>3RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>Tricep Motion of Choice</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>12-15</t>
+        </is>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>1-2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>Optional Bicep Work</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>8-15</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>1-2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="n"/>
+      <c r="D24" s="1" t="n"/>
+      <c r="E24" s="1" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Exercise</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>Sets</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Reps</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>Paused OHP</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="n"/>
+      <c r="C27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n"/>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Chest Supported Row of Choice</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>8-12</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>3RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Paused Larsen Press</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>Lat Pulldowns</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="inlineStr">
+        <is>
+          <t>8-12</t>
+        </is>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
+        <is>
+          <t>3RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n"/>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>Tricep Motion of Choice</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>12-15</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>1-2RIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n"/>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>Rear Delt/Lateral/Front Raise Giant Set</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>8-15</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>2RIR</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B24:E24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>